<commit_message>
Ollama & Openrouter examples
</commit_message>
<xml_diff>
--- a/examples/OpenAI/test_prompts_pdf.xlsx
+++ b/examples/OpenAI/test_prompts_pdf.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Are there any extraneous or ill-fitting pieces of this paper? [paper]</t>
   </si>
   <si>
-    <t xml:space="preserve">Answer in English. Does the following [reply] given any hints for the original language of this paper? [paper]</t>
+    <t xml:space="preserve">Answer in English. Does the following [reply] give any hints for the original language of this paper? [paper]</t>
   </si>
 </sst>
 </file>
@@ -342,7 +342,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Example executable skip test in OpenAI example dir
</commit_message>
<xml_diff>
--- a/examples/OpenAI/test_prompts_pdf.xlsx
+++ b/examples/OpenAI/test_prompts_pdf.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -62,14 +62,26 @@
   </si>
   <si>
     <t xml:space="preserve">Answer in English. Does the following [reply] give any hints for the original language of this paper? [paper]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#py def my_skip_test(answer, param):
+  # some test here making use of the answer
+  Return True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write anything you want!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -137,7 +149,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -147,6 +159,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -339,15 +359,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="49.3"/>
   </cols>
   <sheetData>
@@ -411,6 +432,23 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>